<commit_message>
Added report tooltip and color issue resolved
</commit_message>
<xml_diff>
--- a/documents/Published/Brick Chart/BrickChartByMAQSoftwareChecklist.xlsx
+++ b/documents/Published/Brick Chart/BrickChartByMAQSoftwareChecklist.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18518"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sunny\Desktop\BrickChart\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MAQUser\source\repos\PowerBI-visuals\documents\Published\Brick Chart\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C1B4423-EC3F-4764-A6E5-A6F5BFF51354}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{1AF0E79B-7FE4-4698-B98E-B5963A3F5031}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" xr2:uid="{1AF0E79B-7FE4-4698-B98E-B5963A3F5031}"/>
   </bookViews>
   <sheets>
     <sheet name="BVT" sheetId="1" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="55">
   <si>
     <t>Feature</t>
   </si>
@@ -225,6 +226,52 @@
 6. Update 'Legend name' to 'buyers name'
 7. Update 'Color' to 'black'
 8. Update 'Text size' to '14'</t>
+  </si>
+  <si>
+    <t>Change Data Color</t>
+  </si>
+  <si>
+    <t>1. Go to formatting pane
+2. Go to 'Data Colors'
+3. Update color of first category to 'red'</t>
+  </si>
+  <si>
+    <t>Data Color should be changed to red</t>
+  </si>
+  <si>
+    <t>Gradient</t>
+  </si>
+  <si>
+    <t>Gradient should not be seen in data points</t>
+  </si>
+  <si>
+    <t>Animation</t>
+  </si>
+  <si>
+    <t>1. Go to formatting pane
+2. Toggle 'Animation' to off</t>
+  </si>
+  <si>
+    <t>1. Go to formatting pane
+2. Toggle 'Gradient' to off</t>
+  </si>
+  <si>
+    <t>Animation should be turned off</t>
+  </si>
+  <si>
+    <t>Shape</t>
+  </si>
+  <si>
+    <t>1. Go to formatting pane
+2. Update 'Box shape' to rectangle
+3. Update 'Brick type' to circle</t>
+  </si>
+  <si>
+    <t>1. The shape of the chart should be turned to 'rectangle'
+2. The data points should be dispayed as 'circle'</t>
+  </si>
+  <si>
+    <t>Is Report tooltip working properly?</t>
   </si>
 </sst>
 </file>
@@ -277,7 +324,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -337,11 +384,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFA3A3A3"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFA3A3A3"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFA3A3A3"/>
+      </top>
+      <bottom style="medium">
+        <color theme="0" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color theme="0" tint="-0.249977111117893"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -356,24 +427,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -392,6 +445,38 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -706,17 +791,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6597BE80-5597-4BE2-86EA-034E95536383}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="33.5703125" customWidth="1"/>
     <col min="3" max="3" width="48.42578125" customWidth="1"/>
-    <col min="4" max="4" width="48.28515625" customWidth="1"/>
+    <col min="4" max="4" width="49.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -773,6 +858,62 @@
       </c>
       <c r="D4" s="2" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -782,10 +923,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF2490BC-CF4C-4DE7-A2AC-B86E545BD77C}">
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -970,29 +1111,29 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="6">
-        <v>16</v>
-      </c>
-      <c r="B17" s="15" t="s">
+      <c r="A17" s="13">
+        <v>16</v>
+      </c>
+      <c r="B17" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="16" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="8"/>
-      <c r="B18" s="16" t="s">
+      <c r="A18" s="14"/>
+      <c r="B18" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C18" s="9"/>
+      <c r="C18" s="17"/>
     </row>
     <row r="19" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="10"/>
-      <c r="B19" s="17" t="s">
+      <c r="A19" s="15"/>
+      <c r="B19" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="C19" s="11"/>
+      <c r="C19" s="18"/>
     </row>
     <row r="20" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4">
@@ -1006,41 +1147,41 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="6">
+      <c r="A21" s="13">
         <v>18</v>
       </c>
-      <c r="B21" s="12" t="s">
+      <c r="B21" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="C21" s="16" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="8"/>
-      <c r="B22" s="13" t="s">
+      <c r="A22" s="14"/>
+      <c r="B22" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C22" s="9"/>
+      <c r="C22" s="17"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="8"/>
-      <c r="B23" s="13" t="s">
+      <c r="A23" s="14"/>
+      <c r="B23" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C23" s="9"/>
+      <c r="C23" s="17"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="8"/>
-      <c r="B24" s="13"/>
-      <c r="C24" s="9"/>
+      <c r="A24" s="14"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="17"/>
     </row>
     <row r="25" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="10"/>
-      <c r="B25" s="14" t="s">
+      <c r="A25" s="15"/>
+      <c r="B25" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C25" s="11"/>
+      <c r="C25" s="18"/>
     </row>
     <row r="26" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4">
@@ -1063,6 +1204,22 @@
       <c r="C27" s="5" t="s">
         <v>16</v>
       </c>
+    </row>
+    <row r="28" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="21">
+        <v>21</v>
+      </c>
+      <c r="B28" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="C28" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="20"/>
+      <c r="B29" s="22"/>
+      <c r="C29" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
Fixed JS Exceptions and measure will accept only numeric fields
</commit_message>
<xml_diff>
--- a/documents/Published/Brick Chart/BrickChartByMAQSoftwareChecklist.xlsx
+++ b/documents/Published/Brick Chart/BrickChartByMAQSoftwareChecklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MAQUser\source\repos\PowerBI-visuals\documents\Published\Brick Chart\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PowerBI\GitLab_PowerBI-visuals\documents\Published\Brick Chart\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C1B4423-EC3F-4764-A6E5-A6F5BFF51354}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF5889B9-DF5D-46CF-A6AC-064E06AD0200}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" xr2:uid="{1AF0E79B-7FE4-4698-B98E-B5963A3F5031}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1AF0E79B-7FE4-4698-B98E-B5963A3F5031}"/>
   </bookViews>
   <sheets>
     <sheet name="BVT" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="58">
   <si>
     <t>Feature</t>
   </si>
@@ -272,6 +272,18 @@
   </si>
   <si>
     <t>Is Report tooltip working properly?</t>
+  </si>
+  <si>
+    <t>JS Exception check</t>
+  </si>
+  <si>
+    <t>1. Click on the legend and bricks.
+2. Change the shape of the brick
+3. Click on the spaces between the bricks</t>
+  </si>
+  <si>
+    <t>1. Legend and brick click must cross-filter values in other visuals and the selected bricks must have higher transparency
+2. No console errors must be occurring due to any of the clicks</t>
   </si>
 </sst>
 </file>
@@ -412,7 +424,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -445,38 +457,34 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -791,10 +799,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6597BE80-5597-4BE2-86EA-034E95536383}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -916,8 +924,23 @@
         <v>53</v>
       </c>
     </row>
+    <row r="9" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1111,29 +1134,29 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="13">
+      <c r="A17" s="16">
         <v>16</v>
       </c>
       <c r="B17" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="16" t="s">
+      <c r="C17" s="19" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="14"/>
+      <c r="A18" s="17"/>
       <c r="B18" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C18" s="17"/>
+      <c r="C18" s="20"/>
     </row>
     <row r="19" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="15"/>
+      <c r="A19" s="18"/>
       <c r="B19" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="C19" s="18"/>
+      <c r="C19" s="21"/>
     </row>
     <row r="20" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4">
@@ -1147,41 +1170,41 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="13">
+      <c r="A21" s="16">
         <v>18</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C21" s="16" t="s">
+      <c r="C21" s="19" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="14"/>
+      <c r="A22" s="17"/>
       <c r="B22" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C22" s="17"/>
+      <c r="C22" s="20"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="14"/>
+      <c r="A23" s="17"/>
       <c r="B23" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C23" s="17"/>
+      <c r="C23" s="20"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="14"/>
+      <c r="A24" s="17"/>
       <c r="B24" s="7"/>
-      <c r="C24" s="17"/>
+      <c r="C24" s="20"/>
     </row>
     <row r="25" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="15"/>
+      <c r="A25" s="18"/>
       <c r="B25" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C25" s="18"/>
+      <c r="C25" s="21"/>
     </row>
     <row r="26" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4">
@@ -1206,20 +1229,19 @@
       </c>
     </row>
     <row r="28" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="21">
+      <c r="A28" s="13">
         <v>21</v>
       </c>
-      <c r="B28" s="19" t="s">
+      <c r="B28" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="C28" s="12" t="s">
+      <c r="C28" s="6" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="20"/>
-      <c r="B29" s="22"/>
-      <c r="C29" s="23"/>
+      <c r="B29" s="14"/>
+      <c r="C29" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1229,5 +1251,6 @@
     <mergeCell ref="C21:C25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added context menu Removed typings.json
</commit_message>
<xml_diff>
--- a/documents/Published/Brick Chart/BrickChartByMAQSoftwareChecklist.xlsx
+++ b/documents/Published/Brick Chart/BrickChartByMAQSoftwareChecklist.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PowerBI\GitLab_PowerBI-visuals\documents\Published\Brick Chart\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MAQUser\source\repos\NewRepo2\documents\Published\Brick Chart\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF5889B9-DF5D-46CF-A6AC-064E06AD0200}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A30763E-A21C-4B3A-BF9F-22A7E485BE62}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1AF0E79B-7FE4-4698-B98E-B5963A3F5031}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="61">
   <si>
     <t>Feature</t>
   </si>
@@ -284,6 +284,17 @@
   <si>
     <t>1. Legend and brick click must cross-filter values in other visuals and the selected bricks must have higher transparency
 2. No console errors must be occurring due to any of the clicks</t>
+  </si>
+  <si>
+    <t>Drillthrough</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.Generate a chart with some data
+2.Create new report page and in DrillThrough add the fields for drillthrough.
+3. Right click on the chart, select the Drillthrough option from the menu. </t>
+  </si>
+  <si>
+    <t>1. On right click of the chart and selecting the drillthrough option from the context-menu , the report will drillthrough to the newly created report page.</t>
   </si>
 </sst>
 </file>
@@ -424,7 +435,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -484,6 +495,10 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -799,10 +814,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6597BE80-5597-4BE2-86EA-034E95536383}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="C11" sqref="C11:C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -812,7 +827,7 @@
     <col min="4" max="4" width="49.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -826,7 +841,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -840,7 +855,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -854,7 +869,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="120" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -868,7 +883,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -882,7 +897,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -896,7 +911,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -910,7 +925,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -924,7 +939,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -937,6 +952,21 @@
       <c r="D9" s="2" t="s">
         <v>57</v>
       </c>
+    </row>
+    <row r="10" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A10" s="22">
+        <v>9</v>
+      </c>
+      <c r="B10" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="D10" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="E10" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>